<commit_message>
Extracted data from climate update PDF
</commit_message>
<xml_diff>
--- a/extracted_data/extracted_climate_metdata.xlsx
+++ b/extracted_data/extracted_climate_metdata.xlsx
@@ -273,7 +273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Z249"/>
+  <dimension ref="A1:Z252"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -22026,6 +22026,402 @@
         <v>0</v>
       </c>
     </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>01/07/2025</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Tmax</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>31.9</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>24.1</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>28.5</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>29.9</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>28.8</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>31.3</t>
+        </is>
+      </c>
+      <c r="J250" t="inlineStr">
+        <is>
+          <t>29.4</t>
+        </is>
+      </c>
+      <c r="K250" t="inlineStr">
+        <is>
+          <t>29.3</t>
+        </is>
+      </c>
+      <c r="L250" t="inlineStr">
+        <is>
+          <t>27.3</t>
+        </is>
+      </c>
+      <c r="M250" t="inlineStr">
+        <is>
+          <t>31.2</t>
+        </is>
+      </c>
+      <c r="N250" t="inlineStr">
+        <is>
+          <t>30.4</t>
+        </is>
+      </c>
+      <c r="O250" t="inlineStr">
+        <is>
+          <t>30.6</t>
+        </is>
+      </c>
+      <c r="P250" t="inlineStr">
+        <is>
+          <t>29.0</t>
+        </is>
+      </c>
+      <c r="Q250" t="inlineStr">
+        <is>
+          <t>30.7</t>
+        </is>
+      </c>
+      <c r="R250" t="inlineStr">
+        <is>
+          <t>21.6</t>
+        </is>
+      </c>
+      <c r="S250" t="inlineStr">
+        <is>
+          <t>31.5</t>
+        </is>
+      </c>
+      <c r="T250" t="inlineStr">
+        <is>
+          <t>30.7</t>
+        </is>
+      </c>
+      <c r="U250" t="inlineStr">
+        <is>
+          <t>31.8</t>
+        </is>
+      </c>
+      <c r="V250" t="inlineStr">
+        <is>
+          <t>32.5</t>
+        </is>
+      </c>
+      <c r="W250" t="inlineStr">
+        <is>
+          <t>28.8</t>
+        </is>
+      </c>
+      <c r="X250" t="inlineStr">
+        <is>
+          <t>30.3</t>
+        </is>
+      </c>
+      <c r="Y250" t="inlineStr">
+        <is>
+          <t>31.7</t>
+        </is>
+      </c>
+      <c r="Z250" t="inlineStr">
+        <is>
+          <t>29.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>01/07/2025</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Tmin</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>23.2</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>15.2</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>13.6</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>23.6</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>22.9</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>24.6</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>22.6</t>
+        </is>
+      </c>
+      <c r="J251" t="inlineStr">
+        <is>
+          <t>23.0</t>
+        </is>
+      </c>
+      <c r="K251" t="inlineStr">
+        <is>
+          <t>20.9</t>
+        </is>
+      </c>
+      <c r="L251" t="inlineStr">
+        <is>
+          <t>16.1</t>
+        </is>
+      </c>
+      <c r="M251" t="inlineStr">
+        <is>
+          <t>22.0</t>
+        </is>
+      </c>
+      <c r="N251" t="inlineStr">
+        <is>
+          <t>20.5</t>
+        </is>
+      </c>
+      <c r="O251" t="inlineStr">
+        <is>
+          <t>22.0</t>
+        </is>
+      </c>
+      <c r="P251" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q251" t="inlineStr">
+        <is>
+          <t>22.3</t>
+        </is>
+      </c>
+      <c r="R251" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="S251" t="inlineStr">
+        <is>
+          <t>22.6</t>
+        </is>
+      </c>
+      <c r="T251" t="inlineStr">
+        <is>
+          <t>21.9</t>
+        </is>
+      </c>
+      <c r="U251" t="inlineStr">
+        <is>
+          <t>22.9</t>
+        </is>
+      </c>
+      <c r="V251" t="inlineStr">
+        <is>
+          <t>21.7</t>
+        </is>
+      </c>
+      <c r="W251" t="inlineStr">
+        <is>
+          <t>22.9</t>
+        </is>
+      </c>
+      <c r="X251" t="inlineStr">
+        <is>
+          <t>22.9</t>
+        </is>
+      </c>
+      <c r="Y251" t="inlineStr">
+        <is>
+          <t>21.6</t>
+        </is>
+      </c>
+      <c r="Z251" t="inlineStr">
+        <is>
+          <t>24.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>01/07/2025</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Rainfall</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="M252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="N252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="O252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="P252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="Q252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="R252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="S252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="T252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="U252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="V252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="W252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="X252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="Y252" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="Z252" t="inlineStr">
+        <is>
+          <t>TR</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -22056,396 +22452,396 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="250">
-      <c r="A250" t="inlineStr">
+      <c r="A250" s="2" t="inlineStr">
         <is>
           <t>01/07/2025</t>
         </is>
       </c>
-      <c r="B250" t="inlineStr">
+      <c r="B250" s="2" t="inlineStr">
         <is>
           <t>Tmax</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
+      <c r="C250" s="2" t="inlineStr">
         <is>
           <t>31.9</t>
         </is>
       </c>
-      <c r="D250" t="inlineStr">
+      <c r="D250" s="2" t="inlineStr">
         <is>
           <t>24.1</t>
         </is>
       </c>
-      <c r="E250" t="inlineStr">
+      <c r="E250" s="2" t="inlineStr">
         <is>
           <t>23.9</t>
         </is>
       </c>
-      <c r="F250" t="inlineStr">
+      <c r="F250" s="2" t="inlineStr">
         <is>
           <t>28.5</t>
         </is>
       </c>
-      <c r="G250" t="inlineStr">
+      <c r="G250" s="2" t="inlineStr">
         <is>
           <t>29.9</t>
         </is>
       </c>
-      <c r="H250" t="inlineStr">
+      <c r="H250" s="2" t="inlineStr">
         <is>
           <t>28.8</t>
         </is>
       </c>
-      <c r="I250" t="inlineStr">
+      <c r="I250" s="2" t="inlineStr">
         <is>
           <t>31.3</t>
         </is>
       </c>
-      <c r="J250" t="inlineStr">
+      <c r="J250" s="2" t="inlineStr">
         <is>
           <t>29.4</t>
         </is>
       </c>
-      <c r="K250" t="inlineStr">
+      <c r="K250" s="2" t="inlineStr">
         <is>
           <t>29.3</t>
         </is>
       </c>
-      <c r="L250" t="inlineStr">
+      <c r="L250" s="2" t="inlineStr">
         <is>
           <t>27.3</t>
         </is>
       </c>
-      <c r="M250" t="inlineStr">
+      <c r="M250" s="2" t="inlineStr">
         <is>
           <t>31.2</t>
         </is>
       </c>
-      <c r="N250" t="inlineStr">
+      <c r="N250" s="2" t="inlineStr">
         <is>
           <t>30.4</t>
         </is>
       </c>
-      <c r="O250" t="inlineStr">
+      <c r="O250" s="2" t="inlineStr">
         <is>
           <t>30.6</t>
         </is>
       </c>
-      <c r="P250" t="inlineStr">
+      <c r="P250" s="2" t="inlineStr">
         <is>
           <t>29.0</t>
         </is>
       </c>
-      <c r="Q250" t="inlineStr">
+      <c r="Q250" s="2" t="inlineStr">
         <is>
           <t>30.7</t>
         </is>
       </c>
-      <c r="R250" t="inlineStr">
+      <c r="R250" s="2" t="inlineStr">
         <is>
           <t>21.6</t>
         </is>
       </c>
-      <c r="S250" t="inlineStr">
+      <c r="S250" s="2" t="inlineStr">
         <is>
           <t>31.5</t>
         </is>
       </c>
-      <c r="T250" t="inlineStr">
+      <c r="T250" s="2" t="inlineStr">
         <is>
           <t>30.7</t>
         </is>
       </c>
-      <c r="U250" t="inlineStr">
+      <c r="U250" s="2" t="inlineStr">
         <is>
           <t>31.8</t>
         </is>
       </c>
-      <c r="V250" t="inlineStr">
+      <c r="V250" s="2" t="inlineStr">
         <is>
           <t>32.5</t>
         </is>
       </c>
-      <c r="W250" t="inlineStr">
+      <c r="W250" s="2" t="inlineStr">
         <is>
           <t>28.8</t>
         </is>
       </c>
-      <c r="X250" t="inlineStr">
+      <c r="X250" s="2" t="inlineStr">
         <is>
           <t>30.3</t>
         </is>
       </c>
-      <c r="Y250" t="inlineStr">
+      <c r="Y250" s="2" t="inlineStr">
         <is>
           <t>31.7</t>
         </is>
       </c>
-      <c r="Z250" t="inlineStr">
+      <c r="Z250" s="2" t="inlineStr">
         <is>
           <t>29.2</t>
         </is>
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="inlineStr">
+      <c r="A251" s="2" t="inlineStr">
         <is>
           <t>01/07/2025</t>
         </is>
       </c>
-      <c r="B251" t="inlineStr">
+      <c r="B251" s="2" t="inlineStr">
         <is>
           <t>Tmin</t>
         </is>
       </c>
-      <c r="C251" t="inlineStr">
+      <c r="C251" s="2" t="inlineStr">
         <is>
           <t>23.2</t>
         </is>
       </c>
-      <c r="D251" t="inlineStr">
+      <c r="D251" s="2" t="inlineStr">
         <is>
           <t>15.2</t>
         </is>
       </c>
-      <c r="E251" t="inlineStr">
+      <c r="E251" s="2" t="inlineStr">
         <is>
           <t>13.6</t>
         </is>
       </c>
-      <c r="F251" t="inlineStr">
+      <c r="F251" s="2" t="inlineStr">
         <is>
           <t>23.6</t>
         </is>
       </c>
-      <c r="G251" t="inlineStr">
+      <c r="G251" s="2" t="inlineStr">
         <is>
           <t>22.9</t>
         </is>
       </c>
-      <c r="H251" t="inlineStr">
+      <c r="H251" s="2" t="inlineStr">
         <is>
           <t>24.6</t>
         </is>
       </c>
-      <c r="I251" t="inlineStr">
+      <c r="I251" s="2" t="inlineStr">
         <is>
           <t>22.6</t>
         </is>
       </c>
-      <c r="J251" t="inlineStr">
+      <c r="J251" s="2" t="inlineStr">
         <is>
           <t>23.0</t>
         </is>
       </c>
-      <c r="K251" t="inlineStr">
+      <c r="K251" s="2" t="inlineStr">
         <is>
           <t>20.9</t>
         </is>
       </c>
-      <c r="L251" t="inlineStr">
+      <c r="L251" s="2" t="inlineStr">
         <is>
           <t>16.1</t>
         </is>
       </c>
-      <c r="M251" t="inlineStr">
+      <c r="M251" s="2" t="inlineStr">
         <is>
           <t>22.0</t>
         </is>
       </c>
-      <c r="N251" t="inlineStr">
+      <c r="N251" s="2" t="inlineStr">
         <is>
           <t>20.5</t>
         </is>
       </c>
-      <c r="O251" t="inlineStr">
+      <c r="O251" s="2" t="inlineStr">
         <is>
           <t>22.0</t>
         </is>
       </c>
-      <c r="P251" t="inlineStr">
+      <c r="P251" s="2" t="inlineStr">
         <is>
           <t>25.0</t>
         </is>
       </c>
-      <c r="Q251" t="inlineStr">
+      <c r="Q251" s="2" t="inlineStr">
         <is>
           <t>22.3</t>
         </is>
       </c>
-      <c r="R251" t="inlineStr">
+      <c r="R251" s="2" t="inlineStr">
         <is>
           <t>9.0</t>
         </is>
       </c>
-      <c r="S251" t="inlineStr">
+      <c r="S251" s="2" t="inlineStr">
         <is>
           <t>22.6</t>
         </is>
       </c>
-      <c r="T251" t="inlineStr">
+      <c r="T251" s="2" t="inlineStr">
         <is>
           <t>21.9</t>
         </is>
       </c>
-      <c r="U251" t="inlineStr">
+      <c r="U251" s="2" t="inlineStr">
         <is>
           <t>22.9</t>
         </is>
       </c>
-      <c r="V251" t="inlineStr">
+      <c r="V251" s="2" t="inlineStr">
         <is>
           <t>21.7</t>
         </is>
       </c>
-      <c r="W251" t="inlineStr">
+      <c r="W251" s="2" t="inlineStr">
         <is>
           <t>22.9</t>
         </is>
       </c>
-      <c r="X251" t="inlineStr">
+      <c r="X251" s="2" t="inlineStr">
         <is>
           <t>22.9</t>
         </is>
       </c>
-      <c r="Y251" t="inlineStr">
+      <c r="Y251" s="2" t="inlineStr">
         <is>
           <t>21.6</t>
         </is>
       </c>
-      <c r="Z251" t="inlineStr">
+      <c r="Z251" s="2" t="inlineStr">
         <is>
           <t>24.6</t>
         </is>
       </c>
     </row>
     <row r="252">
-      <c r="A252" t="inlineStr">
+      <c r="A252" s="2" t="inlineStr">
         <is>
           <t>01/07/2025</t>
         </is>
       </c>
-      <c r="B252" t="inlineStr">
+      <c r="B252" s="2" t="inlineStr">
         <is>
           <t>Rainfall</t>
         </is>
       </c>
-      <c r="C252" t="inlineStr">
+      <c r="C252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="D252" t="inlineStr">
+      <c r="D252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="E252" t="inlineStr">
+      <c r="E252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="F252" t="inlineStr">
+      <c r="F252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="G252" t="inlineStr">
+      <c r="G252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="H252" t="inlineStr">
+      <c r="H252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="I252" t="inlineStr">
+      <c r="I252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="J252" t="inlineStr">
+      <c r="J252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="K252" t="inlineStr">
+      <c r="K252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L252" t="inlineStr">
+      <c r="L252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="M252" t="inlineStr">
+      <c r="M252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="N252" t="inlineStr">
+      <c r="N252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="O252" t="inlineStr">
+      <c r="O252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="P252" t="inlineStr">
+      <c r="P252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="Q252" t="inlineStr">
+      <c r="Q252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="R252" t="inlineStr">
+      <c r="R252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="S252" t="inlineStr">
+      <c r="S252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="T252" t="inlineStr">
+      <c r="T252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="U252" t="inlineStr">
+      <c r="U252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="V252" t="inlineStr">
+      <c r="V252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="W252" t="inlineStr">
+      <c r="W252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="X252" t="inlineStr">
+      <c r="X252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="Y252" t="inlineStr">
+      <c r="Y252" s="2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="Z252" t="inlineStr">
+      <c r="Z252" s="2" t="inlineStr">
         <is>
           <t>TR</t>
         </is>

</xml_diff>